<commit_message>
change design to 4 layer PCB
</commit_message>
<xml_diff>
--- a/Documantation/PIN_MAPPING_PX30.xlsx
+++ b/Documantation/PIN_MAPPING_PX30.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="423">
   <si>
     <t xml:space="preserve">Pin # PX30</t>
   </si>
@@ -743,9 +743,6 @@
   </si>
   <si>
     <t xml:space="preserve">T DM_SDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPIO3_C4_d</t>
   </si>
   <si>
     <t xml:space="preserve">CODEC_I2S_SDOUT</t>
@@ -1553,12 +1550,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1624,19 +1621,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L56" activeCellId="0" sqref="L56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.19"/>
@@ -1651,7 +1647,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,22 +3395,22 @@
         <v>240</v>
       </c>
       <c r="G60" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H60" s="17" t="s">
         <v>241</v>
-      </c>
-      <c r="H60" s="17" t="s">
-        <v>242</v>
       </c>
       <c r="I60" s="15" t="n">
         <v>118</v>
       </c>
       <c r="J60" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="K60" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="K60" s="8" t="s">
+      <c r="L60" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="L60" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="O60" s="16"/>
     </row>
@@ -3424,37 +3419,37 @@
         <v>119</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="D61" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="E61" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="F61" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="G61" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="G61" s="8" t="s">
+      <c r="H61" s="17" t="s">
         <v>251</v>
-      </c>
-      <c r="H61" s="17" t="s">
-        <v>252</v>
       </c>
       <c r="I61" s="15" t="n">
         <v>120</v>
       </c>
       <c r="J61" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="K61" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="K61" s="8" t="s">
+      <c r="L61" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="L61" s="8" t="s">
-        <v>255</v>
       </c>
       <c r="O61" s="16"/>
     </row>
@@ -3500,13 +3495,13 @@
         <v>124</v>
       </c>
       <c r="J63" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="K63" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="K63" s="8" t="s">
+      <c r="L63" s="8" t="s">
         <v>257</v>
-      </c>
-      <c r="L63" s="8" t="s">
-        <v>258</v>
       </c>
       <c r="O63" s="16"/>
     </row>
@@ -3527,19 +3522,19 @@
         <v>126</v>
       </c>
       <c r="J64" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="K64" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="K64" s="8" t="s">
+      <c r="L64" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="L64" s="8" t="s">
+      <c r="M64" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="M64" s="8" t="s">
+      <c r="N64" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="N64" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="O64" s="16"/>
     </row>
@@ -3560,19 +3555,19 @@
         <v>128</v>
       </c>
       <c r="J65" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="K65" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="K65" s="8" t="s">
+      <c r="L65" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="L65" s="8" t="s">
+      <c r="M65" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="M65" s="8" t="s">
+      <c r="N65" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="N65" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="O65" s="16"/>
     </row>
@@ -3593,19 +3588,19 @@
         <v>130</v>
       </c>
       <c r="J66" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="K66" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="K66" s="8" t="s">
+      <c r="L66" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="L66" s="8" t="s">
+      <c r="M66" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="M66" s="8" t="s">
+      <c r="N66" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="N66" s="8" t="s">
-        <v>273</v>
       </c>
       <c r="O66" s="16"/>
     </row>
@@ -3639,25 +3634,25 @@
         <v>133</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="H68" s="17" t="s">
         <v>274</v>
-      </c>
-      <c r="H68" s="17" t="s">
-        <v>275</v>
       </c>
       <c r="I68" s="15" t="n">
         <v>134</v>
       </c>
       <c r="J68" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="K68" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="K68" s="8" t="s">
+      <c r="L68" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="L68" s="8" t="s">
+      <c r="M68" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="M68" s="8" t="s">
-        <v>279</v>
       </c>
       <c r="O68" s="16"/>
     </row>
@@ -3666,28 +3661,28 @@
         <v>135</v>
       </c>
       <c r="B69" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H69" s="17" t="s">
         <v>280</v>
-      </c>
-      <c r="H69" s="17" t="s">
-        <v>281</v>
       </c>
       <c r="I69" s="15" t="n">
         <v>136</v>
       </c>
       <c r="J69" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="K69" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="K69" s="8" t="s">
+      <c r="L69" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="L69" s="8" t="s">
+      <c r="M69" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="M69" s="8" t="s">
+      <c r="N69" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="N69" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="O69" s="16"/>
     </row>
@@ -3708,16 +3703,16 @@
         <v>138</v>
       </c>
       <c r="J70" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="K70" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="K70" s="8" t="s">
+      <c r="L70" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="L70" s="8" t="s">
+      <c r="M70" s="8" t="s">
         <v>289</v>
-      </c>
-      <c r="M70" s="8" t="s">
-        <v>290</v>
       </c>
       <c r="O70" s="16"/>
     </row>
@@ -3738,16 +3733,16 @@
         <v>140</v>
       </c>
       <c r="J71" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="K71" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="K71" s="8" t="s">
+      <c r="L71" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="L71" s="8" t="s">
+      <c r="M71" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="M71" s="8" t="s">
-        <v>294</v>
       </c>
       <c r="O71" s="16"/>
     </row>
@@ -3768,16 +3763,16 @@
         <v>142</v>
       </c>
       <c r="J72" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="K72" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="K72" s="8" t="s">
+      <c r="L72" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="L72" s="8" t="s">
+      <c r="M72" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="M72" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="O72" s="16"/>
     </row>
@@ -3798,19 +3793,19 @@
         <v>144</v>
       </c>
       <c r="J73" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="K73" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="K73" s="8" t="s">
+      <c r="L73" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="L73" s="8" t="s">
+      <c r="M73" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="M73" s="8" t="s">
+      <c r="N73" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="N73" s="8" t="s">
-        <v>303</v>
       </c>
       <c r="O73" s="16"/>
     </row>
@@ -3819,28 +3814,28 @@
         <v>145</v>
       </c>
       <c r="B74" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H74" s="17" t="s">
         <v>304</v>
-      </c>
-      <c r="H74" s="17" t="s">
-        <v>305</v>
       </c>
       <c r="I74" s="15" t="n">
         <v>146</v>
       </c>
       <c r="J74" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="K74" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="K74" s="8" t="s">
+      <c r="L74" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="L74" s="8" t="s">
+      <c r="M74" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="M74" s="8" t="s">
+      <c r="N74" s="8" t="s">
         <v>309</v>
-      </c>
-      <c r="N74" s="8" t="s">
-        <v>310</v>
       </c>
       <c r="O74" s="16"/>
     </row>
@@ -3861,19 +3856,19 @@
         <v>148</v>
       </c>
       <c r="J75" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="K75" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="K75" s="8" t="s">
+      <c r="L75" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="L75" s="8" t="s">
+      <c r="M75" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="M75" s="8" t="s">
+      <c r="N75" s="8" t="s">
         <v>314</v>
-      </c>
-      <c r="N75" s="8" t="s">
-        <v>315</v>
       </c>
       <c r="O75" s="16"/>
     </row>
@@ -3894,7 +3889,7 @@
         <v>150</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O76" s="16"/>
     </row>
@@ -3915,10 +3910,10 @@
         <v>152</v>
       </c>
       <c r="J77" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="O77" s="16" t="s">
         <v>317</v>
-      </c>
-      <c r="O77" s="16" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3938,7 +3933,7 @@
         <v>154</v>
       </c>
       <c r="J78" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="O78" s="16"/>
     </row>
@@ -3959,10 +3954,10 @@
         <v>156</v>
       </c>
       <c r="J79" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="K79" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="K79" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="O79" s="16"/>
     </row>
@@ -3983,10 +3978,10 @@
         <v>158</v>
       </c>
       <c r="J80" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="K80" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="K80" s="8" t="s">
-        <v>323</v>
       </c>
       <c r="O80" s="16"/>
     </row>
@@ -4007,13 +4002,13 @@
         <v>160</v>
       </c>
       <c r="J81" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="K81" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="K81" s="8" t="s">
+      <c r="L81" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="L81" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="O81" s="16"/>
     </row>
@@ -4034,13 +4029,13 @@
         <v>162</v>
       </c>
       <c r="J82" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="K82" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="K82" s="8" t="s">
+      <c r="L82" s="8" t="s">
         <v>328</v>
-      </c>
-      <c r="L82" s="8" t="s">
-        <v>329</v>
       </c>
       <c r="O82" s="16"/>
     </row>
@@ -4061,13 +4056,13 @@
         <v>164</v>
       </c>
       <c r="J83" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="K83" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="K83" s="8" t="s">
+      <c r="L83" s="8" t="s">
         <v>331</v>
-      </c>
-      <c r="L83" s="8" t="s">
-        <v>332</v>
       </c>
       <c r="O83" s="16"/>
     </row>
@@ -4088,13 +4083,13 @@
         <v>166</v>
       </c>
       <c r="J84" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="K84" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="K84" s="8" t="s">
+      <c r="L84" s="8" t="s">
         <v>334</v>
-      </c>
-      <c r="L84" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="O84" s="16"/>
     </row>
@@ -4115,13 +4110,13 @@
         <v>168</v>
       </c>
       <c r="J85" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="K85" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="K85" s="8" t="s">
+      <c r="L85" s="8" t="s">
         <v>337</v>
-      </c>
-      <c r="L85" s="8" t="s">
-        <v>338</v>
       </c>
       <c r="O85" s="16"/>
     </row>
@@ -4142,13 +4137,13 @@
         <v>170</v>
       </c>
       <c r="J86" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="K86" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="K86" s="8" t="s">
+      <c r="L86" s="8" t="s">
         <v>340</v>
-      </c>
-      <c r="L86" s="8" t="s">
-        <v>341</v>
       </c>
       <c r="O86" s="16"/>
     </row>
@@ -4169,13 +4164,13 @@
         <v>172</v>
       </c>
       <c r="J87" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="K87" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="K87" s="8" t="s">
+      <c r="L87" s="8" t="s">
         <v>343</v>
-      </c>
-      <c r="L87" s="8" t="s">
-        <v>344</v>
       </c>
       <c r="O87" s="16"/>
     </row>
@@ -4196,13 +4191,13 @@
         <v>174</v>
       </c>
       <c r="J88" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="K88" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="K88" s="8" t="s">
+      <c r="L88" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="L88" s="8" t="s">
-        <v>347</v>
       </c>
       <c r="O88" s="16"/>
     </row>
@@ -4223,13 +4218,13 @@
         <v>176</v>
       </c>
       <c r="J89" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="K89" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="K89" s="8" t="s">
+      <c r="L89" s="8" t="s">
         <v>349</v>
-      </c>
-      <c r="L89" s="8" t="s">
-        <v>350</v>
       </c>
       <c r="O89" s="16"/>
     </row>
@@ -4250,13 +4245,13 @@
         <v>178</v>
       </c>
       <c r="J90" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="K90" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="K90" s="8" t="s">
+      <c r="L90" s="8" t="s">
         <v>352</v>
-      </c>
-      <c r="L90" s="8" t="s">
-        <v>353</v>
       </c>
       <c r="O90" s="16"/>
     </row>
@@ -4265,7 +4260,7 @@
         <v>179</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H91" s="9"/>
       <c r="I91" s="6" t="n">
@@ -4285,20 +4280,20 @@
         <v>181</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H92" s="9"/>
       <c r="I92" s="15" t="n">
         <v>182</v>
       </c>
       <c r="J92" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="K92" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="K92" s="8" t="s">
+      <c r="L92" s="8" t="s">
         <v>357</v>
-      </c>
-      <c r="L92" s="8" t="s">
-        <v>358</v>
       </c>
       <c r="O92" s="16"/>
     </row>
@@ -4307,20 +4302,20 @@
         <v>183</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H93" s="9"/>
       <c r="I93" s="15" t="n">
         <v>184</v>
       </c>
       <c r="J93" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="K93" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="K93" s="8" t="s">
+      <c r="L93" s="8" t="s">
         <v>361</v>
-      </c>
-      <c r="L93" s="8" t="s">
-        <v>362</v>
       </c>
       <c r="O93" s="16"/>
     </row>
@@ -4362,13 +4357,13 @@
         <v>188</v>
       </c>
       <c r="J95" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="K95" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="K95" s="8" t="s">
+      <c r="L95" s="8" t="s">
         <v>364</v>
-      </c>
-      <c r="L95" s="8" t="s">
-        <v>365</v>
       </c>
       <c r="O95" s="16"/>
     </row>
@@ -4414,13 +4409,13 @@
         <v>192</v>
       </c>
       <c r="J97" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="K97" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="K97" s="8" t="s">
+      <c r="L97" s="8" t="s">
         <v>367</v>
-      </c>
-      <c r="L97" s="8" t="s">
-        <v>368</v>
       </c>
       <c r="O97" s="16"/>
     </row>
@@ -4441,13 +4436,13 @@
         <v>194</v>
       </c>
       <c r="J98" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="K98" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="K98" s="8" t="s">
+      <c r="L98" s="8" t="s">
         <v>370</v>
-      </c>
-      <c r="L98" s="8" t="s">
-        <v>371</v>
       </c>
       <c r="O98" s="16"/>
     </row>
@@ -4481,7 +4476,7 @@
         <v>197</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G100" s="21"/>
       <c r="H100" s="9"/>
@@ -4489,13 +4484,13 @@
         <v>198</v>
       </c>
       <c r="J100" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="K100" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="K100" s="8" t="s">
+      <c r="L100" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="L100" s="8" t="s">
-        <v>375</v>
       </c>
       <c r="O100" s="16"/>
     </row>
@@ -4504,7 +4499,7 @@
         <v>199</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G101" s="21"/>
       <c r="H101" s="9"/>
@@ -4525,7 +4520,7 @@
         <v>201</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G102" s="21"/>
       <c r="H102" s="9"/>
@@ -4533,13 +4528,13 @@
         <v>202</v>
       </c>
       <c r="J102" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="K102" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="K102" s="8" t="s">
+      <c r="L102" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="L102" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="O102" s="16"/>
     </row>
@@ -4548,7 +4543,7 @@
         <v>203</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G103" s="21"/>
       <c r="H103" s="9"/>
@@ -4556,13 +4551,13 @@
         <v>204</v>
       </c>
       <c r="J103" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="K103" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="K103" s="8" t="s">
+      <c r="L103" s="8" t="s">
         <v>383</v>
-      </c>
-      <c r="L103" s="8" t="s">
-        <v>384</v>
       </c>
       <c r="O103" s="16"/>
     </row>
@@ -4596,16 +4591,16 @@
         <v>207</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="D105" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="E105" s="8" t="s">
         <v>387</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>388</v>
       </c>
       <c r="G105" s="21"/>
       <c r="H105" s="9"/>
@@ -4626,16 +4621,16 @@
         <v>209</v>
       </c>
       <c r="B106" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="D106" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="D106" s="8" t="s">
+      <c r="E106" s="8" t="s">
         <v>391</v>
-      </c>
-      <c r="E106" s="8" t="s">
-        <v>392</v>
       </c>
       <c r="G106" s="21"/>
       <c r="H106" s="9"/>
@@ -4643,13 +4638,13 @@
         <v>210</v>
       </c>
       <c r="J106" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="K106" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="K106" s="8" t="s">
+      <c r="L106" s="8" t="s">
         <v>394</v>
-      </c>
-      <c r="L106" s="8" t="s">
-        <v>395</v>
       </c>
       <c r="O106" s="16"/>
     </row>
@@ -4670,13 +4665,13 @@
         <v>212</v>
       </c>
       <c r="J107" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="K107" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="K107" s="8" t="s">
+      <c r="L107" s="8" t="s">
         <v>397</v>
-      </c>
-      <c r="L107" s="8" t="s">
-        <v>398</v>
       </c>
       <c r="O107" s="16"/>
     </row>
@@ -4722,10 +4717,10 @@
         <v>216</v>
       </c>
       <c r="J109" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="K109" s="8" t="s">
         <v>399</v>
-      </c>
-      <c r="K109" s="8" t="s">
-        <v>400</v>
       </c>
       <c r="O109" s="16"/>
     </row>
@@ -4746,10 +4741,10 @@
         <v>218</v>
       </c>
       <c r="J110" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="K110" s="8" t="s">
         <v>401</v>
-      </c>
-      <c r="K110" s="8" t="s">
-        <v>402</v>
       </c>
       <c r="O110" s="16"/>
     </row>
@@ -4770,7 +4765,7 @@
         <v>220</v>
       </c>
       <c r="J111" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="O111" s="16"/>
     </row>
@@ -4779,7 +4774,7 @@
         <v>221</v>
       </c>
       <c r="B112" s="24" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C112" s="23"/>
       <c r="D112" s="23"/>
@@ -4804,7 +4799,7 @@
         <v>223</v>
       </c>
       <c r="B113" s="24" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C113" s="23"/>
       <c r="D113" s="23"/>
@@ -4829,7 +4824,7 @@
         <v>225</v>
       </c>
       <c r="B114" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C114" s="23"/>
       <c r="D114" s="23"/>
@@ -4841,7 +4836,7 @@
         <v>226</v>
       </c>
       <c r="J114" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K114" s="23"/>
       <c r="L114" s="23"/>
@@ -4854,7 +4849,7 @@
         <v>227</v>
       </c>
       <c r="B115" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C115" s="23"/>
       <c r="D115" s="23"/>
@@ -4866,7 +4861,7 @@
         <v>228</v>
       </c>
       <c r="J115" s="24" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K115" s="23"/>
       <c r="L115" s="23"/>
@@ -4879,7 +4874,7 @@
         <v>229</v>
       </c>
       <c r="B116" s="24" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C116" s="23"/>
       <c r="D116" s="23"/>
@@ -4916,7 +4911,7 @@
         <v>232</v>
       </c>
       <c r="J117" s="24" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K117" s="23"/>
       <c r="L117" s="23"/>
@@ -4929,7 +4924,7 @@
         <v>233</v>
       </c>
       <c r="B118" s="24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C118" s="23"/>
       <c r="D118" s="23"/>
@@ -4941,7 +4936,7 @@
         <v>234</v>
       </c>
       <c r="J118" s="24" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K118" s="23"/>
       <c r="L118" s="23"/>
@@ -4954,7 +4949,7 @@
         <v>235</v>
       </c>
       <c r="B119" s="24" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C119" s="23"/>
       <c r="D119" s="23"/>
@@ -4979,7 +4974,7 @@
         <v>237</v>
       </c>
       <c r="B120" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C120" s="23"/>
       <c r="D120" s="23"/>
@@ -4991,7 +4986,7 @@
         <v>238</v>
       </c>
       <c r="J120" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K120" s="23"/>
       <c r="L120" s="23"/>
@@ -5004,7 +4999,7 @@
         <v>239</v>
       </c>
       <c r="B121" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C121" s="23"/>
       <c r="D121" s="23"/>
@@ -5154,7 +5149,7 @@
         <v>251</v>
       </c>
       <c r="B127" s="24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C127" s="23"/>
       <c r="D127" s="23"/>
@@ -5166,7 +5161,7 @@
         <v>252</v>
       </c>
       <c r="J127" s="24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K127" s="23"/>
       <c r="L127" s="23"/>
@@ -5179,7 +5174,7 @@
         <v>253</v>
       </c>
       <c r="B128" s="24" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C128" s="23"/>
       <c r="D128" s="23"/>
@@ -5191,7 +5186,7 @@
         <v>254</v>
       </c>
       <c r="J128" s="24" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K128" s="23"/>
       <c r="L128" s="23"/>
@@ -5204,7 +5199,7 @@
         <v>255</v>
       </c>
       <c r="B129" s="24" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C129" s="23"/>
       <c r="D129" s="23"/>
@@ -5216,7 +5211,7 @@
         <v>256</v>
       </c>
       <c r="J129" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K129" s="23"/>
       <c r="L129" s="23"/>
@@ -5229,7 +5224,7 @@
         <v>257</v>
       </c>
       <c r="B130" s="24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C130" s="23"/>
       <c r="D130" s="23"/>
@@ -5241,7 +5236,7 @@
         <v>258</v>
       </c>
       <c r="J130" s="24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K130" s="23"/>
       <c r="L130" s="23"/>
@@ -5254,7 +5249,7 @@
         <v>259</v>
       </c>
       <c r="B131" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C131" s="23"/>
       <c r="D131" s="23"/>
@@ -5266,7 +5261,7 @@
         <v>260</v>
       </c>
       <c r="J131" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K131" s="23"/>
       <c r="L131" s="23"/>

</xml_diff>